<commit_message>
modified dataset and recalculated
</commit_message>
<xml_diff>
--- a/eclipse/correlation/correlation_eclipse_1.xlsx
+++ b/eclipse/correlation/correlation_eclipse_1.xlsx
@@ -471,31 +471,36 @@
           <t>0.00318</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.06531</t>
+        </is>
       </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.002509191178027626</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>332.4375</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
         <v>3</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>36</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>332.4375</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>108</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>105</v>
       </c>
     </row>
@@ -523,31 +528,36 @@
           <t>0.06578</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.06283</t>
+        </is>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.001227683302393919</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>1843.863888888889</v>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>2</v>
       </c>
       <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
         <v>1843.863888888889</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>2</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>11</v>
       </c>
     </row>
@@ -575,31 +585,36 @@
           <t>0.04703</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0.05101</t>
+        </is>
       </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.0002400367742999085</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>235.6991666666667</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>12.90322580645161</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>1</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>2</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>235.6991666666667</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>6</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>8</v>
       </c>
     </row>
@@ -627,31 +642,36 @@
           <t>0.00286</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.06187</t>
+        </is>
       </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.002828833316241492</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>443.4619444444444</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>5.555555555555555</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>4</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>443.4619444444444</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>12</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>12</v>
       </c>
     </row>
@@ -679,31 +699,36 @@
           <t>0.00277</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0.06323</t>
+        </is>
       </c>
       <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.004669213427387585</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>449.2013888888889</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>2</v>
       </c>
       <c r="L7" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" t="n">
         <v>449.2013888888889</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>4</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>6</v>
       </c>
     </row>
@@ -731,31 +756,36 @@
           <t>0.00010</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0.06323</t>
+        </is>
       </c>
       <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.001838297862340467</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>518.7630555555555</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
       <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
         <v>2</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>6</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>518.7630555555555</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>15</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>18</v>
       </c>
     </row>
@@ -783,31 +813,36 @@
           <t>0.06682</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0.06569</t>
+        </is>
       </c>
       <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.003815216863170928</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>514.8277777777778</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>8.333333333333332</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>4</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>11</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>514.8277777777778</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>33</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>36</v>
       </c>
     </row>
@@ -835,31 +870,36 @@
           <t>0.01095</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>0</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.06147</t>
+        </is>
       </c>
       <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.001029206300910475</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>588.2583333333333</v>
       </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
         <v>588.2583333333333</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>3</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>3</v>
       </c>
     </row>
@@ -887,31 +927,36 @@
           <t>0.07668</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>0</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.06501</t>
+        </is>
       </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.008016427397947317</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>682.1633333333333</v>
       </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>2</v>
       </c>
       <c r="L11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M11" t="n">
         <v>682.1633333333333</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>4</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>6</v>
       </c>
     </row>
@@ -939,31 +984,36 @@
           <t>0.06682</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>0</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0.06283</t>
+        </is>
       </c>
       <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.0002851381189280918</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>411.4547222222222</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>11.76470588235294</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
       </c>
       <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
         <v>411.4547222222222</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>5</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -991,31 +1041,36 @@
           <t>0.00367</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>0</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0.06187</t>
+        </is>
       </c>
       <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.001124243348095551</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>419.9575</v>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
       </c>
       <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
         <v>419.9575</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>3</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1043,31 +1098,36 @@
           <t>0.01095</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>0</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0.03690</t>
+        </is>
       </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.0002237013143944748</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>393.9983333333333</v>
       </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
         <v>393.9983333333333</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>3</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>